<commit_message>
feat: operational cost analysis egg production feature
</commit_message>
<xml_diff>
--- a/data/Research_Data.xlsx
+++ b/data/Research_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pramudi\Desktop\Research\Pramudi\data-set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA6108-58BB-4406-84B5-AEBC1DC5B6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823B081A-37E7-4A31-A2F0-5D40FF519778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{42D074F0-E98E-4DF9-8CA8-53ADD03A5FDB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42D074F0-E98E-4DF9-8CA8-53ADD03A5FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feed Consumption" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="DOC price Range" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="97">
   <si>
     <t>f_died_count</t>
   </si>
@@ -308,9 +307,6 @@
     <t>Other costs(Maintenance)</t>
   </si>
   <si>
-    <t>0.31 or user input</t>
-  </si>
-  <si>
     <t>Rs/egg based on Harti 2023</t>
   </si>
   <si>
@@ -330,6 +326,12 @@
   </si>
   <si>
     <t>livability</t>
+  </si>
+  <si>
+    <t>small_egg_lay_per</t>
+  </si>
+  <si>
+    <t>egg_loss</t>
   </si>
 </sst>
 </file>
@@ -472,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -567,11 +569,62 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8.8000000000000007"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8.8000000000000007"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1302,41 +1355,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7E4D4895-054A-436D-90AB-EAC3878C6EBB}" name="Table6" displayName="Table6" ref="A1:I102" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42">
-  <autoFilter ref="A1:I102" xr:uid="{7E4D4895-054A-436D-90AB-EAC3878C6EBB}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B9DF78B5-1B34-419D-8AE3-009EA3E99EBD}" name="week" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{F7F6C682-1CB2-4D02-BCD9-6BB91E8986FB}" name="feed_type" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{1A98F0F4-CF72-475D-BCAB-A4DA06571D64}" name="std_weight" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{AD77A9C3-02DE-44BE-82C1-1073C856C01A}" name="feed" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{F8ACE035-668B-48FB-A9BA-C69B63DEDEF6}" name="gain" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{61D76B7A-67EA-4D64-938F-7C6659A6D511}" name="laying_per" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{0B3197FD-1C3E-4E54-8534-B0BEB423C492}" name="egg_weight" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{84B5B5DC-2610-4F01-BD8F-F5FF1F53C2C8}" name="fcr" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{08C61A6B-3210-4585-8F6D-90E7A376EC14}" name="livability" dataDxfId="32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7E4D4895-054A-436D-90AB-EAC3878C6EBB}" name="Table6" displayName="Table6" ref="A1:K102" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44">
+  <autoFilter ref="A1:K102" xr:uid="{7E4D4895-054A-436D-90AB-EAC3878C6EBB}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{B9DF78B5-1B34-419D-8AE3-009EA3E99EBD}" name="week" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{F7F6C682-1CB2-4D02-BCD9-6BB91E8986FB}" name="feed_type" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{1A98F0F4-CF72-475D-BCAB-A4DA06571D64}" name="std_weight" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{AD77A9C3-02DE-44BE-82C1-1073C856C01A}" name="feed" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{F8ACE035-668B-48FB-A9BA-C69B63DEDEF6}" name="gain" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{61D76B7A-67EA-4D64-938F-7C6659A6D511}" name="laying_per" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{0B3197FD-1C3E-4E54-8534-B0BEB423C492}" name="egg_weight" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{84B5B5DC-2610-4F01-BD8F-F5FF1F53C2C8}" name="fcr" dataDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{08C61A6B-3210-4585-8F6D-90E7A376EC14}" name="livability" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{62D46C20-5D0B-4ED2-A419-43C169473E95}" name="small_egg_lay_per" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{AF3FE821-EB70-4C2B-AF75-77342BC83239}" name="egg_loss" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2DBF409-4AC3-40FD-9896-C56A9ECD31DB}" name="Table3" displayName="Table3" ref="A1:L1386" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2DBF409-4AC3-40FD-9896-C56A9ECD31DB}" name="Table3" displayName="Table3" ref="A1:L1386" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32">
   <autoFilter ref="A1:L1386" xr:uid="{D2DBF409-4AC3-40FD-9896-C56A9ECD31DB}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{4A3A0ACF-5093-46A4-9CF8-DD50EB99AD08}" name="ddate" totalsRowLabel="Total" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{3141688A-9A36-458E-B84E-AD1DACC3942A}" name="week_no" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{C5D29ED2-F951-419C-931E-32030AE3C9C0}" name="female_count" totalsRowFunction="custom" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{4A3A0ACF-5093-46A4-9CF8-DD50EB99AD08}" name="ddate" totalsRowLabel="Total" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{3141688A-9A36-458E-B84E-AD1DACC3942A}" name="week_no" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{C5D29ED2-F951-419C-931E-32030AE3C9C0}" name="female_count" totalsRowFunction="custom" dataDxfId="28">
       <totalsRowFormula>SUM(C2:C1386)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DA30C84B-1A14-4220-990F-C0655503B56F}" name="f_died_count" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{65F66F89-7183-47EC-885F-92BCF7B6E314}" name="f_cul_count" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{A6FF9FD9-5E38-4334-9C70-A84978B22293}" name="female_feed" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{C3E8D4BE-D895-4CF4-BB85-65C762ABCB12}" name="egg_small" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{AFAEE9B9-D7A4-4556-B18E-B108B1EE5534}" name="egg_broken" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{965B9439-6015-418F-8C02-FEB7050D0CCC}" name="egg_shell" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{947E7646-FAA9-4E46-AFFF-1F2AAC4B8DE2}" name="white_eggs" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{7B6759E3-AA06-431A-BCCB-E3100BF0896F}" name="brown_eggs" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{7545B8F3-DECF-4EA7-94EE-A269CCB09BC1}" name="egg_weight" totalsRowFunction="sum" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{DA30C84B-1A14-4220-990F-C0655503B56F}" name="f_died_count" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{65F66F89-7183-47EC-885F-92BCF7B6E314}" name="f_cul_count" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{A6FF9FD9-5E38-4334-9C70-A84978B22293}" name="female_feed" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{C3E8D4BE-D895-4CF4-BB85-65C762ABCB12}" name="egg_small" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{AFAEE9B9-D7A4-4556-B18E-B108B1EE5534}" name="egg_broken" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{965B9439-6015-418F-8C02-FEB7050D0CCC}" name="egg_shell" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{947E7646-FAA9-4E46-AFFF-1F2AAC4B8DE2}" name="white_eggs" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{7B6759E3-AA06-431A-BCCB-E3100BF0896F}" name="brown_eggs" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{7545B8F3-DECF-4EA7-94EE-A269CCB09BC1}" name="egg_weight" totalsRowFunction="sum" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1346,17 +1401,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86B4CA98-E04B-4690-A4F2-F55954441B7E}" name="price_table" displayName="price_table" ref="A1:I51" totalsRowShown="0">
   <autoFilter ref="A1:I51" xr:uid="{86B4CA98-E04B-4690-A4F2-F55954441B7E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FBA9C3B5-65CD-41E5-A083-3D56328A6FE5}" name="Year" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{8F38A280-79A1-4E49-A3BC-8E3953AF885C}" name="Month" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{73DE41BE-073B-44DB-8907-BBA6F9238A2C}" name="Brown Egg Price" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{1669F886-BFA6-46A5-9C90-DD752E06369A}" name=" White Egg Price" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{CE50030B-A5C7-4E1B-9A83-74D0B2B36ED1}" name="Farm egg small price" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{FBA9C3B5-65CD-41E5-A083-3D56328A6FE5}" name="Year" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{8F38A280-79A1-4E49-A3BC-8E3953AF885C}" name="Month" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{73DE41BE-073B-44DB-8907-BBA6F9238A2C}" name="Brown Egg Price" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{1669F886-BFA6-46A5-9C90-DD752E06369A}" name=" White Egg Price" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{CE50030B-A5C7-4E1B-9A83-74D0B2B36ED1}" name="Farm egg small price" dataDxfId="14">
       <calculatedColumnFormula>(price_table[[#This Row],[ White Egg Price]]-3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3F6EDB2C-C5E6-46FF-96D0-BEF700677EAE}" name="DOC price Avg" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{34677460-AEB4-4875-8FE0-0D5C178F3595}" name="Feed Starter Price/kg" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{306ABBA0-A2B7-4660-AB40-F08F67C678A6}" name="Feed Grower Price /kg" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{DE7E37E6-F9C1-4B0F-8E6E-4559B43A06B7}" name="Feed Layer Price/kg" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{3F6EDB2C-C5E6-46FF-96D0-BEF700677EAE}" name="DOC price Avg" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{34677460-AEB4-4875-8FE0-0D5C178F3595}" name="Feed Starter Price/kg" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{306ABBA0-A2B7-4660-AB40-F08F67C678A6}" name="Feed Grower Price /kg" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{DE7E37E6-F9C1-4B0F-8E6E-4559B43A06B7}" name="Feed Layer Price/kg" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1366,10 +1421,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{84BF7CD8-FD56-472C-A5AE-228C2C730423}" name="Table5" displayName="Table5" ref="A1:D645" totalsRowShown="0">
   <autoFilter ref="A1:D645" xr:uid="{84BF7CD8-FD56-472C-A5AE-228C2C730423}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5E211683-BC08-4085-A2A4-DAC9E7E69E61}" name="Date" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F2F6B2F8-1325-4E95-AA9B-930C1307A0E3}" name="From (Rs)" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{B1DCA9A9-2CA5-452C-87C7-7F8F9062076C}" name="To(Rs)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{2C90F4BB-A6F6-410F-887E-88D7B587F202}" name="Avg Price " dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{5E211683-BC08-4085-A2A4-DAC9E7E69E61}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{F2F6B2F8-1325-4E95-AA9B-930C1307A0E3}" name="From (Rs)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{B1DCA9A9-2CA5-452C-87C7-7F8F9062076C}" name="To(Rs)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{2C90F4BB-A6F6-410F-887E-88D7B587F202}" name="Avg Price " dataDxfId="6">
       <calculatedColumnFormula>(Table5[[#This Row],[From (Rs)]]+Table5[[#This Row],[To(Rs)]])/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1378,18 +1433,18 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0F856A8A-2FB1-4516-BA6E-29477B9B4256}" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0F856A8A-2FB1-4516-BA6E-29477B9B4256}" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:B6" xr:uid="{0F856A8A-2FB1-4516-BA6E-29477B9B4256}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8DEDEEB5-2E6C-4548-9BF2-712F004A04C5}" name="Cost Item" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{1714A15C-64A3-4607-AB2D-19F86A91A44D}" name="Rs/egg based on Harti 2023" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{8DEDEEB5-2E6C-4548-9BF2-712F004A04C5}" name="Cost Item" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1714A15C-64A3-4607-AB2D-19F86A91A44D}" name="Rs/egg based on Harti 2023" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5F2F961D-896E-411B-8473-EDC4EF0584BF}" name="Table7" displayName="Table7" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5F2F961D-896E-411B-8473-EDC4EF0584BF}" name="Table7" displayName="Table7" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:A1048576" xr:uid="{5F2F961D-896E-411B-8473-EDC4EF0584BF}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{BD5B6003-6B6F-4D4B-8DA7-E8C4007B7016}" name="DOC price Range"/>
@@ -1715,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F705B95E-A4AE-4A2E-BB43-C07BD60CDD1F}">
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,9 +1786,11 @@
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -1756,18 +1813,24 @@
         <v>8</v>
       </c>
       <c r="H1" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
+      <c r="K1" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="O1" s="7"/>
       <c r="P1" s="32"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1789,16 +1852,25 @@
       <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
       <c r="I2" s="4">
         <v>100</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="31"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1820,15 +1892,23 @@
       <c r="G3" s="4">
         <v>0</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
       <c r="I3" s="4">
         <v>100</v>
       </c>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
       <c r="P3" s="31"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1850,15 +1930,24 @@
       <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
       <c r="I4" s="4">
         <v>100</v>
       </c>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="34"/>
       <c r="P4" s="31"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1880,15 +1969,23 @@
       <c r="G5" s="4">
         <v>0</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
       <c r="I5" s="4">
         <v>100</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
       <c r="P5" s="31"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1910,15 +2007,24 @@
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
       <c r="I6" s="4">
         <v>100</v>
       </c>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="34"/>
       <c r="P6" s="31"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1940,15 +2046,23 @@
       <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
       <c r="I7" s="4">
         <v>100</v>
       </c>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
       <c r="P7" s="31"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1970,15 +2084,24 @@
       <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
       <c r="I8" s="4">
         <v>100</v>
       </c>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="34"/>
       <c r="P8" s="31"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2000,15 +2123,23 @@
       <c r="G9" s="4">
         <v>0</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
       <c r="I9" s="4">
         <v>100</v>
       </c>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
       <c r="P9" s="31"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2030,15 +2161,23 @@
       <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
       <c r="I10" s="4">
         <v>100</v>
       </c>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
       <c r="P10" s="31"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2060,15 +2199,23 @@
       <c r="G11" s="4">
         <v>0</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
       <c r="I11" s="4">
         <v>100</v>
       </c>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
       <c r="P11" s="31"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2090,15 +2237,23 @@
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
       <c r="I12" s="4">
         <v>100</v>
       </c>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
       <c r="P12" s="31"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2120,15 +2275,23 @@
       <c r="G13" s="4">
         <v>0</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
       <c r="I13" s="4">
         <v>100</v>
       </c>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
       <c r="P13" s="31"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2150,15 +2313,23 @@
       <c r="G14" s="2">
         <v>0</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
       <c r="I14" s="4">
         <v>100</v>
       </c>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
       <c r="P14" s="31"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2180,15 +2351,23 @@
       <c r="G15" s="4">
         <v>0</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
       <c r="I15" s="4">
         <v>100</v>
       </c>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
       <c r="P15" s="31"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2210,15 +2389,23 @@
       <c r="G16" s="2">
         <v>0</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
       <c r="I16" s="4">
         <v>100</v>
       </c>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
       <c r="P16" s="31"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2240,15 +2427,23 @@
       <c r="G17" s="4">
         <v>0</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
       <c r="I17" s="4">
         <v>100</v>
       </c>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
       <c r="P17" s="31"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2270,15 +2465,23 @@
       <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
       <c r="I18" s="4">
         <v>100</v>
       </c>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
       <c r="P18" s="31"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2306,11 +2509,18 @@
       <c r="I19" s="31">
         <v>99.9</v>
       </c>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
+      <c r="J19" s="4">
+        <f>AVERAGE(20,25)</f>
+        <v>22.5</v>
+      </c>
+      <c r="K19">
+        <v>0.8</v>
+      </c>
       <c r="P19" s="31"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2338,11 +2548,18 @@
       <c r="I20" s="4">
         <v>99.8</v>
       </c>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
+      <c r="J20" s="4">
+        <f t="shared" ref="J20:J21" si="0">AVERAGE(20,25)</f>
+        <v>22.5</v>
+      </c>
+      <c r="K20">
+        <v>0.8</v>
+      </c>
       <c r="P20" s="31"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2370,11 +2587,18 @@
       <c r="I21" s="4">
         <v>99.8</v>
       </c>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
+      <c r="J21" s="4">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="K21">
+        <v>0.8</v>
+      </c>
       <c r="P21" s="31"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2402,11 +2626,18 @@
       <c r="I22" s="4">
         <v>99.7</v>
       </c>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
+      <c r="J22" s="4">
+        <f>AVERAGE(10,15)</f>
+        <v>12.5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P22" s="31"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2434,11 +2665,18 @@
       <c r="I23" s="4">
         <v>99.6</v>
       </c>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
+      <c r="J23" s="4">
+        <f>AVERAGE(10,15)</f>
+        <v>12.5</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P23" s="31"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2466,11 +2704,18 @@
       <c r="I24" s="4">
         <v>99.5</v>
       </c>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
+      <c r="J24" s="4">
+        <f>AVERAGE(5,10)</f>
+        <v>7.5</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P24" s="31"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2498,11 +2743,18 @@
       <c r="I25" s="4">
         <v>99.5</v>
       </c>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
+      <c r="J25" s="4">
+        <f>AVERAGE(5,10)</f>
+        <v>7.5</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P25" s="31"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2530,11 +2782,17 @@
       <c r="I26" s="4">
         <v>99.4</v>
       </c>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
+      <c r="J26" s="4">
+        <v>5</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P26" s="31"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2562,11 +2820,17 @@
       <c r="I27" s="4">
         <v>99.3</v>
       </c>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
+      <c r="J27" s="4">
+        <v>5</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P27" s="31"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2594,11 +2858,17 @@
       <c r="I28" s="4">
         <v>99.2</v>
       </c>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
+      <c r="J28" s="4">
+        <v>5</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P28" s="31"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2626,11 +2896,17 @@
       <c r="I29" s="4">
         <v>99.1</v>
       </c>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
+      <c r="J29" s="4">
+        <v>4</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P29" s="31"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2658,11 +2934,17 @@
       <c r="I30" s="4">
         <v>99.1</v>
       </c>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
+      <c r="J30" s="4">
+        <v>4</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P30" s="31"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2690,11 +2972,17 @@
       <c r="I31" s="4">
         <v>99</v>
       </c>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
+      <c r="J31" s="4">
+        <v>5</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P31" s="31"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2722,11 +3010,17 @@
       <c r="I32" s="4">
         <v>98.9</v>
       </c>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
+      <c r="J32" s="4">
+        <v>3</v>
+      </c>
+      <c r="K32" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P32" s="31"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2754,11 +3048,17 @@
       <c r="I33" s="4">
         <v>98.8</v>
       </c>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
+      <c r="J33" s="4">
+        <v>2</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0.4</v>
+      </c>
       <c r="P33" s="31"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q33" s="31"/>
+      <c r="R33" s="31"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2786,11 +3086,17 @@
       <c r="I34" s="4">
         <v>98.8</v>
       </c>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
+      <c r="J34" s="4">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P34" s="31"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -2818,11 +3124,17 @@
       <c r="I35" s="4">
         <v>98.7</v>
       </c>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
+      <c r="J35" s="4">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P35" s="31"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q35" s="31"/>
+      <c r="R35" s="31"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2850,11 +3162,17 @@
       <c r="I36" s="4">
         <v>98.6</v>
       </c>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
+      <c r="J36" s="4">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P36" s="31"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q36" s="31"/>
+      <c r="R36" s="31"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2882,11 +3200,17 @@
       <c r="I37" s="4">
         <v>98.5</v>
       </c>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
+      <c r="J37" s="4">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P37" s="31"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2914,11 +3238,17 @@
       <c r="I38" s="4">
         <v>98.4</v>
       </c>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
+      <c r="J38" s="4">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P38" s="31"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -2946,11 +3276,17 @@
       <c r="I39" s="4">
         <v>98.4</v>
       </c>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
+      <c r="J39" s="4">
+        <v>0</v>
+      </c>
+      <c r="K39" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P39" s="31"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2978,11 +3314,17 @@
       <c r="I40" s="4">
         <v>98.3</v>
       </c>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
+      <c r="J40" s="4">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P40" s="31"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q40" s="31"/>
+      <c r="R40" s="31"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3010,11 +3352,17 @@
       <c r="I41" s="4">
         <v>98.2</v>
       </c>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
+      <c r="J41" s="4">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P41" s="31"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3042,11 +3390,17 @@
       <c r="I42" s="4">
         <v>98.1</v>
       </c>
-      <c r="N42" s="31"/>
-      <c r="O42" s="31"/>
+      <c r="J42" s="4">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P42" s="31"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -3074,11 +3428,17 @@
       <c r="I43" s="4">
         <v>98</v>
       </c>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
+      <c r="J43" s="4">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P43" s="31"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q43" s="31"/>
+      <c r="R43" s="31"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3106,11 +3466,17 @@
       <c r="I44" s="4">
         <v>98</v>
       </c>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31"/>
+      <c r="J44" s="4">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P44" s="31"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q44" s="31"/>
+      <c r="R44" s="31"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -3138,11 +3504,17 @@
       <c r="I45" s="4">
         <v>97.9</v>
       </c>
-      <c r="N45" s="31"/>
-      <c r="O45" s="31"/>
+      <c r="J45" s="4">
+        <v>0</v>
+      </c>
+      <c r="K45" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P45" s="31"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q45" s="31"/>
+      <c r="R45" s="31"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3170,11 +3542,17 @@
       <c r="I46" s="4">
         <v>97.8</v>
       </c>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31"/>
+      <c r="J46" s="4">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P46" s="31"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -3202,11 +3580,17 @@
       <c r="I47" s="4">
         <v>97.7</v>
       </c>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
+      <c r="J47" s="4">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P47" s="31"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q47" s="31"/>
+      <c r="R47" s="31"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3234,11 +3618,17 @@
       <c r="I48" s="4">
         <v>97.7</v>
       </c>
-      <c r="N48" s="31"/>
-      <c r="O48" s="31"/>
+      <c r="J48" s="4">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P48" s="31"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q48" s="31"/>
+      <c r="R48" s="31"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -3266,11 +3656,17 @@
       <c r="I49" s="4">
         <v>97.6</v>
       </c>
-      <c r="N49" s="31"/>
-      <c r="O49" s="31"/>
+      <c r="J49" s="4">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P49" s="31"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3298,11 +3694,17 @@
       <c r="I50" s="4">
         <v>97.5</v>
       </c>
-      <c r="N50" s="31"/>
-      <c r="O50" s="31"/>
+      <c r="J50" s="4">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P50" s="31"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q50" s="31"/>
+      <c r="R50" s="31"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -3330,11 +3732,17 @@
       <c r="I51" s="4">
         <v>97.4</v>
       </c>
-      <c r="N51" s="31"/>
-      <c r="O51" s="31"/>
+      <c r="J51" s="4">
+        <v>0</v>
+      </c>
+      <c r="K51" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P51" s="31"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q51" s="31"/>
+      <c r="R51" s="31"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3362,11 +3770,17 @@
       <c r="I52" s="4">
         <v>97.3</v>
       </c>
-      <c r="N52" s="31"/>
-      <c r="O52" s="31"/>
+      <c r="J52" s="4">
+        <v>0</v>
+      </c>
+      <c r="K52" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P52" s="31"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q52" s="31"/>
+      <c r="R52" s="31"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -3394,11 +3808,17 @@
       <c r="I53" s="4">
         <v>97.3</v>
       </c>
-      <c r="N53" s="31"/>
-      <c r="O53" s="31"/>
+      <c r="J53" s="4">
+        <v>0</v>
+      </c>
+      <c r="K53" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P53" s="31"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q53" s="31"/>
+      <c r="R53" s="31"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -3426,11 +3846,17 @@
       <c r="I54" s="4">
         <v>97.2</v>
       </c>
-      <c r="N54" s="31"/>
-      <c r="O54" s="31"/>
+      <c r="J54" s="4">
+        <v>0</v>
+      </c>
+      <c r="K54" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P54" s="31"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q54" s="31"/>
+      <c r="R54" s="31"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -3458,11 +3884,17 @@
       <c r="I55" s="4">
         <v>97.1</v>
       </c>
-      <c r="N55" s="31"/>
-      <c r="O55" s="31"/>
+      <c r="J55" s="4">
+        <v>0</v>
+      </c>
+      <c r="K55" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P55" s="31"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q55" s="31"/>
+      <c r="R55" s="31"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -3490,11 +3922,17 @@
       <c r="I56" s="4">
         <v>97</v>
       </c>
-      <c r="N56" s="31"/>
-      <c r="O56" s="31"/>
+      <c r="J56" s="4">
+        <v>0</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P56" s="31"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q56" s="31"/>
+      <c r="R56" s="31"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -3522,11 +3960,17 @@
       <c r="I57" s="4">
         <v>97</v>
       </c>
-      <c r="N57" s="31"/>
-      <c r="O57" s="31"/>
+      <c r="J57" s="4">
+        <v>0</v>
+      </c>
+      <c r="K57" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P57" s="31"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q57" s="31"/>
+      <c r="R57" s="31"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3554,12 +3998,18 @@
       <c r="I58" s="4">
         <v>96.9</v>
       </c>
-      <c r="M58" s="24"/>
-      <c r="N58" s="31"/>
-      <c r="O58" s="31"/>
+      <c r="J58" s="4">
+        <v>0</v>
+      </c>
+      <c r="K58" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O58" s="24"/>
       <c r="P58" s="31"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q58" s="31"/>
+      <c r="R58" s="31"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -3587,12 +4037,18 @@
       <c r="I59" s="4">
         <v>96.8</v>
       </c>
-      <c r="M59" s="30"/>
-      <c r="N59" s="31"/>
-      <c r="O59" s="31"/>
+      <c r="J59" s="4">
+        <v>0</v>
+      </c>
+      <c r="K59" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O59" s="30"/>
       <c r="P59" s="31"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q59" s="31"/>
+      <c r="R59" s="31"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3620,12 +4076,18 @@
       <c r="I60" s="4">
         <v>96.7</v>
       </c>
-      <c r="M60" s="30"/>
-      <c r="N60" s="31"/>
-      <c r="O60" s="31"/>
+      <c r="J60" s="4">
+        <v>0</v>
+      </c>
+      <c r="K60" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O60" s="30"/>
       <c r="P60" s="31"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q60" s="31"/>
+      <c r="R60" s="31"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -3653,12 +4115,18 @@
       <c r="I61" s="4">
         <v>96.6</v>
       </c>
-      <c r="M61" s="30"/>
-      <c r="N61" s="31"/>
-      <c r="O61" s="31"/>
+      <c r="J61" s="4">
+        <v>0</v>
+      </c>
+      <c r="K61" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O61" s="30"/>
       <c r="P61" s="31"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q61" s="31"/>
+      <c r="R61" s="31"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3686,12 +4154,18 @@
       <c r="I62" s="4">
         <v>96.6</v>
       </c>
-      <c r="M62" s="30"/>
-      <c r="N62" s="31"/>
-      <c r="O62" s="31"/>
+      <c r="J62" s="4">
+        <v>0</v>
+      </c>
+      <c r="K62" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O62" s="30"/>
       <c r="P62" s="31"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q62" s="31"/>
+      <c r="R62" s="31"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -3719,12 +4193,18 @@
       <c r="I63" s="4">
         <v>96.5</v>
       </c>
-      <c r="M63" s="30"/>
-      <c r="N63" s="31"/>
-      <c r="O63" s="31"/>
+      <c r="J63" s="4">
+        <v>0</v>
+      </c>
+      <c r="K63" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O63" s="30"/>
       <c r="P63" s="31"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q63" s="31"/>
+      <c r="R63" s="31"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -3752,12 +4232,18 @@
       <c r="I64" s="4">
         <v>96.4</v>
       </c>
-      <c r="M64" s="30"/>
-      <c r="N64" s="31"/>
-      <c r="O64" s="31"/>
+      <c r="J64" s="4">
+        <v>0</v>
+      </c>
+      <c r="K64" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O64" s="30"/>
       <c r="P64" s="31"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q64" s="31"/>
+      <c r="R64" s="31"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -3785,12 +4271,18 @@
       <c r="I65" s="4">
         <v>96.3</v>
       </c>
-      <c r="M65" s="30"/>
-      <c r="N65" s="31"/>
-      <c r="O65" s="31"/>
+      <c r="J65" s="4">
+        <v>0</v>
+      </c>
+      <c r="K65" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O65" s="30"/>
       <c r="P65" s="31"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q65" s="31"/>
+      <c r="R65" s="31"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -3818,12 +4310,18 @@
       <c r="I66" s="4">
         <v>96.3</v>
       </c>
-      <c r="M66" s="30"/>
-      <c r="N66" s="31"/>
-      <c r="O66" s="31"/>
+      <c r="J66" s="4">
+        <v>0</v>
+      </c>
+      <c r="K66" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O66" s="30"/>
       <c r="P66" s="31"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q66" s="31"/>
+      <c r="R66" s="31"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -3851,12 +4349,18 @@
       <c r="I67" s="4">
         <v>96.2</v>
       </c>
-      <c r="M67" s="30"/>
-      <c r="N67" s="31"/>
-      <c r="O67" s="31"/>
+      <c r="J67" s="4">
+        <v>0</v>
+      </c>
+      <c r="K67" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O67" s="30"/>
       <c r="P67" s="31"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q67" s="31"/>
+      <c r="R67" s="31"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -3884,12 +4388,18 @@
       <c r="I68" s="4">
         <v>96.1</v>
       </c>
-      <c r="M68" s="30"/>
-      <c r="N68" s="31"/>
-      <c r="O68" s="31"/>
+      <c r="J68" s="4">
+        <v>0</v>
+      </c>
+      <c r="K68" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O68" s="30"/>
       <c r="P68" s="31"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q68" s="31"/>
+      <c r="R68" s="31"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -3917,12 +4427,18 @@
       <c r="I69" s="4">
         <v>96</v>
       </c>
-      <c r="M69" s="30"/>
-      <c r="N69" s="31"/>
-      <c r="O69" s="31"/>
+      <c r="J69" s="4">
+        <v>0</v>
+      </c>
+      <c r="K69" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O69" s="30"/>
       <c r="P69" s="31"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q69" s="31"/>
+      <c r="R69" s="31"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -3950,12 +4466,18 @@
       <c r="I70" s="4">
         <v>95.9</v>
       </c>
-      <c r="M70" s="30"/>
-      <c r="N70" s="31"/>
-      <c r="O70" s="31"/>
+      <c r="J70" s="4">
+        <v>0</v>
+      </c>
+      <c r="K70" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O70" s="30"/>
       <c r="P70" s="31"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q70" s="31"/>
+      <c r="R70" s="31"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -3983,12 +4505,18 @@
       <c r="I71" s="4">
         <v>95.9</v>
       </c>
-      <c r="M71" s="30"/>
-      <c r="N71" s="31"/>
-      <c r="O71" s="31"/>
+      <c r="J71" s="4">
+        <v>0</v>
+      </c>
+      <c r="K71" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O71" s="30"/>
       <c r="P71" s="31"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q71" s="31"/>
+      <c r="R71" s="31"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -4016,12 +4544,18 @@
       <c r="I72" s="4">
         <v>95.8</v>
       </c>
-      <c r="M72" s="30"/>
-      <c r="N72" s="31"/>
-      <c r="O72" s="31"/>
+      <c r="J72" s="4">
+        <v>0</v>
+      </c>
+      <c r="K72" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O72" s="30"/>
       <c r="P72" s="31"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q72" s="31"/>
+      <c r="R72" s="31"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -4049,12 +4583,18 @@
       <c r="I73" s="4">
         <v>95.7</v>
       </c>
-      <c r="M73" s="30"/>
-      <c r="N73" s="31"/>
-      <c r="O73" s="31"/>
+      <c r="J73" s="4">
+        <v>0</v>
+      </c>
+      <c r="K73" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O73" s="30"/>
       <c r="P73" s="31"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q73" s="31"/>
+      <c r="R73" s="31"/>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -4082,12 +4622,18 @@
       <c r="I74" s="4">
         <v>95.6</v>
       </c>
-      <c r="M74" s="30"/>
-      <c r="N74" s="31"/>
-      <c r="O74" s="31"/>
+      <c r="J74" s="4">
+        <v>0</v>
+      </c>
+      <c r="K74" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O74" s="30"/>
       <c r="P74" s="31"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q74" s="31"/>
+      <c r="R74" s="31"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -4115,12 +4661,18 @@
       <c r="I75" s="4">
         <v>95.6</v>
       </c>
-      <c r="M75" s="30"/>
-      <c r="N75" s="31"/>
-      <c r="O75" s="31"/>
+      <c r="J75" s="4">
+        <v>0</v>
+      </c>
+      <c r="K75" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O75" s="30"/>
       <c r="P75" s="31"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q75" s="31"/>
+      <c r="R75" s="31"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -4148,12 +4700,18 @@
       <c r="I76" s="4">
         <v>95.5</v>
       </c>
-      <c r="M76" s="30"/>
-      <c r="N76" s="31"/>
-      <c r="O76" s="31"/>
+      <c r="J76" s="4">
+        <v>0</v>
+      </c>
+      <c r="K76" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O76" s="30"/>
       <c r="P76" s="31"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q76" s="31"/>
+      <c r="R76" s="31"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -4181,12 +4739,18 @@
       <c r="I77" s="4">
         <v>95.4</v>
       </c>
-      <c r="M77" s="30"/>
-      <c r="N77" s="31"/>
-      <c r="O77" s="31"/>
+      <c r="J77" s="4">
+        <v>0</v>
+      </c>
+      <c r="K77" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O77" s="30"/>
       <c r="P77" s="31"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q77" s="31"/>
+      <c r="R77" s="31"/>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -4214,12 +4778,18 @@
       <c r="I78" s="4">
         <v>95.3</v>
       </c>
-      <c r="M78" s="30"/>
-      <c r="N78" s="31"/>
-      <c r="O78" s="31"/>
+      <c r="J78" s="4">
+        <v>0</v>
+      </c>
+      <c r="K78" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O78" s="30"/>
       <c r="P78" s="31"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q78" s="31"/>
+      <c r="R78" s="31"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -4247,12 +4817,18 @@
       <c r="I79" s="4">
         <v>95.2</v>
       </c>
-      <c r="M79" s="30"/>
-      <c r="N79" s="31"/>
-      <c r="O79" s="31"/>
+      <c r="J79" s="4">
+        <v>0</v>
+      </c>
+      <c r="K79" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="O79" s="30"/>
       <c r="P79" s="31"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q79" s="31"/>
+      <c r="R79" s="31"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -4280,11 +4856,17 @@
       <c r="I80" s="4">
         <v>95.2</v>
       </c>
-      <c r="N80" s="31"/>
-      <c r="O80" s="31"/>
+      <c r="J80" s="4">
+        <v>0</v>
+      </c>
+      <c r="K80" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P80" s="31"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q80" s="31"/>
+      <c r="R80" s="31"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -4312,11 +4894,17 @@
       <c r="I81" s="4">
         <v>95.1</v>
       </c>
-      <c r="N81" s="31"/>
-      <c r="O81" s="31"/>
+      <c r="J81" s="4">
+        <v>0</v>
+      </c>
+      <c r="K81" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P81" s="31"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q81" s="31"/>
+      <c r="R81" s="31"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -4344,11 +4932,17 @@
       <c r="I82" s="4">
         <v>95</v>
       </c>
-      <c r="N82" s="31"/>
-      <c r="O82" s="31"/>
+      <c r="J82" s="4">
+        <v>0</v>
+      </c>
+      <c r="K82" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P82" s="31"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q82" s="31"/>
+      <c r="R82" s="31"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -4376,11 +4970,17 @@
       <c r="I83" s="4">
         <v>94.9</v>
       </c>
-      <c r="N83" s="31"/>
-      <c r="O83" s="31"/>
+      <c r="J83" s="4">
+        <v>0</v>
+      </c>
+      <c r="K83" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P83" s="31"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q83" s="31"/>
+      <c r="R83" s="31"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -4408,11 +5008,17 @@
       <c r="I84" s="4">
         <v>94.9</v>
       </c>
-      <c r="N84" s="31"/>
-      <c r="O84" s="31"/>
+      <c r="J84" s="4">
+        <v>0</v>
+      </c>
+      <c r="K84" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P84" s="31"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q84" s="31"/>
+      <c r="R84" s="31"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -4440,11 +5046,17 @@
       <c r="I85" s="4">
         <v>94.8</v>
       </c>
-      <c r="N85" s="31"/>
-      <c r="O85" s="31"/>
+      <c r="J85" s="4">
+        <v>0</v>
+      </c>
+      <c r="K85" s="4">
+        <v>0.6</v>
+      </c>
       <c r="P85" s="31"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q85" s="31"/>
+      <c r="R85" s="31"/>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -4472,8 +5084,14 @@
       <c r="I86" s="4">
         <v>94.7</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J86" s="4">
+        <v>0</v>
+      </c>
+      <c r="K86" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -4501,8 +5119,14 @@
       <c r="I87" s="4">
         <v>94.6</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J87" s="4">
+        <v>0</v>
+      </c>
+      <c r="K87" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -4530,8 +5154,14 @@
       <c r="I88" s="4">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J88" s="4">
+        <v>0</v>
+      </c>
+      <c r="K88" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -4559,8 +5189,14 @@
       <c r="I89" s="4">
         <v>93.7</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J89" s="4">
+        <v>0</v>
+      </c>
+      <c r="K89" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -4588,8 +5224,14 @@
       <c r="I90" s="4">
         <v>93.6</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J90" s="4">
+        <v>0</v>
+      </c>
+      <c r="K90" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -4617,8 +5259,14 @@
       <c r="I91" s="4">
         <v>94.3</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J91" s="4">
+        <v>0</v>
+      </c>
+      <c r="K91" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -4646,8 +5294,14 @@
       <c r="I92" s="4">
         <v>94.2</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J92" s="4">
+        <v>0</v>
+      </c>
+      <c r="K92" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -4675,8 +5329,14 @@
       <c r="I93" s="4">
         <v>94.1</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J93" s="4">
+        <v>0</v>
+      </c>
+      <c r="K93" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -4704,8 +5364,14 @@
       <c r="I94" s="4">
         <v>94.1</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J94" s="4">
+        <v>0</v>
+      </c>
+      <c r="K94" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -4733,8 +5399,14 @@
       <c r="I95" s="4">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J95" s="4">
+        <v>0</v>
+      </c>
+      <c r="K95" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -4762,8 +5434,14 @@
       <c r="I96" s="4">
         <v>93.9</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J96" s="4">
+        <v>0</v>
+      </c>
+      <c r="K96" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -4791,8 +5469,14 @@
       <c r="I97" s="4">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J97" s="4">
+        <v>0</v>
+      </c>
+      <c r="K97" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -4820,8 +5504,14 @@
       <c r="I98" s="4">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J98" s="4">
+        <v>0</v>
+      </c>
+      <c r="K98" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -4849,8 +5539,14 @@
       <c r="I99" s="4">
         <v>93.7</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J99" s="4">
+        <v>0</v>
+      </c>
+      <c r="K99" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -4878,8 +5574,14 @@
       <c r="I100" s="4">
         <v>93.6</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J100" s="4">
+        <v>0</v>
+      </c>
+      <c r="K100" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -4907,8 +5609,14 @@
       <c r="I101" s="4">
         <v>93.5</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J101" s="4">
+        <v>0</v>
+      </c>
+      <c r="K101" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -4918,6 +5626,8 @@
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4931,8 +5641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03133343-D906-40FC-806C-AEE63469B4D2}">
   <dimension ref="A1:L1386"/>
   <sheetViews>
-    <sheetView topLeftCell="A1139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K706" sqref="K706"/>
+    <sheetView topLeftCell="A684" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A698" sqref="A698:XFD704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9929,7 +10639,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>44496</v>
       </c>
@@ -57632,8 +58342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155DFC1F-97B4-4B33-B749-BFC44F958B37}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59264,7 +59974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D7078D-8B8C-43DE-88E9-110BD3002FCD}">
   <dimension ref="A1:D645"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -59280,16 +59990,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -68965,7 +69675,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68979,7 +69689,7 @@
         <v>82</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -69010,8 +69720,8 @@
       <c r="A5" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>88</v>
+      <c r="B5" s="23">
+        <v>0.31</v>
       </c>
       <c r="D5" s="6"/>
     </row>

</xml_diff>